<commit_message>
product interface document update
</commit_message>
<xml_diff>
--- a/工程接口说明文档.xlsx
+++ b/工程接口说明文档.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21029"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\65499\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ideaWorkSpaces\项目相关文档\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AEEFF4C-0CAF-4B4E-AD62-F4CBECC68132}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12540" tabRatio="735" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="930" yWindow="0" windowWidth="28800" windowHeight="12540" tabRatio="735" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="idm(用户信息管理系统)" sheetId="2" r:id="rId1"/>
-    <sheet name="appBackEnd(手机app后台)" sheetId="1" r:id="rId2"/>
-    <sheet name="PushMsgService(消息推送中心)" sheetId="3" r:id="rId3"/>
+    <sheet name="ACV-UA" sheetId="2" r:id="rId1"/>
+    <sheet name="ACV-NA" sheetId="3" r:id="rId2"/>
+    <sheet name="ACV-VA" sheetId="1" r:id="rId3"/>
     <sheet name="SmartSpeakerService(智能音箱后台服务)" sheetId="4" r:id="rId4"/>
     <sheet name="EmspSvc(Powershare后台服务接口)" sheetId="5" r:id="rId5"/>
     <sheet name="CarModelIOT()" sheetId="6" r:id="rId6"/>
@@ -273,7 +272,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -618,25 +617,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.44140625" customWidth="1"/>
-    <col min="2" max="2" width="14.77734375" customWidth="1"/>
-    <col min="3" max="3" width="64.109375" customWidth="1"/>
-    <col min="4" max="4" width="17.109375" customWidth="1"/>
+    <col min="1" max="1" width="17.4140625" customWidth="1"/>
+    <col min="2" max="2" width="14.75" customWidth="1"/>
+    <col min="3" max="3" width="64.08203125" customWidth="1"/>
+    <col min="4" max="4" width="17.08203125" customWidth="1"/>
     <col min="5" max="5" width="13.33203125" customWidth="1"/>
     <col min="6" max="6" width="20" customWidth="1"/>
-    <col min="11" max="11" width="17.109375" customWidth="1"/>
+    <col min="11" max="11" width="17.08203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="39.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="39.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -653,7 +652,7 @@
       <c r="J1" s="6"/>
       <c r="K1" s="6"/>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
         <v>2</v>
       </c>
@@ -670,7 +669,7 @@
       <c r="J2" s="7"/>
       <c r="K2" s="7"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="10"/>
       <c r="B3" s="7" t="s">
         <v>4</v>
@@ -685,7 +684,7 @@
       <c r="J3" s="7"/>
       <c r="K3" s="7"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="11" t="s">
         <v>5</v>
       </c>
@@ -703,7 +702,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="11"/>
       <c r="B5" t="s">
         <v>10</v>
@@ -712,7 +711,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="11"/>
       <c r="C6" t="s">
         <v>12</v>
@@ -722,7 +721,7 @@
       </c>
       <c r="F6" s="11"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="11"/>
       <c r="C7" t="s">
         <v>14</v>
@@ -732,7 +731,7 @@
       </c>
       <c r="F7" s="11"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" s="11"/>
       <c r="C8" t="s">
         <v>15</v>
@@ -742,7 +741,7 @@
       </c>
       <c r="F8" s="11"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="11"/>
       <c r="C9" t="s">
         <v>16</v>
@@ -752,7 +751,7 @@
       </c>
       <c r="F9" s="11"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="11"/>
       <c r="C10" t="s">
         <v>17</v>
@@ -762,7 +761,7 @@
       </c>
       <c r="F10" s="11"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="11"/>
       <c r="C11" t="s">
         <v>18</v>
@@ -772,7 +771,7 @@
       </c>
       <c r="F11" s="11"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" s="11"/>
       <c r="C12" t="s">
         <v>19</v>
@@ -782,7 +781,7 @@
       </c>
       <c r="F12" s="11"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" s="11"/>
       <c r="C13" t="s">
         <v>20</v>
@@ -792,18 +791,18 @@
       </c>
       <c r="F13" s="11"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" s="11"/>
       <c r="F14" s="11"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" s="11"/>
       <c r="B15" t="s">
         <v>21</v>
       </c>
       <c r="F15" s="11"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" s="11"/>
       <c r="C16" t="s">
         <v>22</v>
@@ -813,7 +812,7 @@
       </c>
       <c r="F16" s="11"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="11"/>
       <c r="C17" t="s">
         <v>23</v>
@@ -823,7 +822,7 @@
       </c>
       <c r="F17" s="11"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="11"/>
       <c r="C18" t="s">
         <v>24</v>
@@ -833,7 +832,7 @@
       </c>
       <c r="F18" s="11"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="11"/>
       <c r="C19" t="s">
         <v>25</v>
@@ -843,14 +842,14 @@
       </c>
       <c r="F19" s="11"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="11"/>
       <c r="B20" t="s">
         <v>26</v>
       </c>
       <c r="F20" s="11"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="11"/>
       <c r="C21" t="s">
         <v>27</v>
@@ -860,7 +859,7 @@
       </c>
       <c r="F21" s="11"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="11"/>
       <c r="C22" t="s">
         <v>28</v>
@@ -882,10 +881,10 @@
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E5 E15 E20" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E5 E15 E20">
       <formula1>"是,否"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E16 E17 E18 E19 E21 E22 E6:E14" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E16 E17 E18 E19 E21 E22 E6:E14">
       <formula1>"√,×"</formula1>
     </dataValidation>
   </dataValidations>
@@ -894,30 +893,31 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:K27"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L3" sqref="A3:XFD3"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.77734375" customWidth="1"/>
-    <col min="2" max="2" width="40.44140625" customWidth="1"/>
-    <col min="3" max="3" width="67.109375" customWidth="1"/>
-    <col min="4" max="4" width="15.44140625" customWidth="1"/>
-    <col min="5" max="5" width="16.77734375" customWidth="1"/>
-    <col min="6" max="6" width="30.44140625" customWidth="1"/>
-    <col min="13" max="15" width="8.6640625" customWidth="1"/>
+    <col min="1" max="1" width="23.33203125" customWidth="1"/>
+    <col min="2" max="2" width="25" customWidth="1"/>
+    <col min="3" max="3" width="64.75" customWidth="1"/>
+    <col min="4" max="4" width="25.25" customWidth="1"/>
+    <col min="5" max="5" width="18.25" customWidth="1"/>
+    <col min="6" max="6" width="32.33203125" customWidth="1"/>
+    <col min="7" max="7" width="22.58203125" customWidth="1"/>
+    <col min="11" max="11" width="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="31.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>29</v>
+        <v>70</v>
       </c>
       <c r="C1" s="6"/>
       <c r="D1" s="6"/>
@@ -929,12 +929,12 @@
       <c r="J1" s="6"/>
       <c r="K1" s="6"/>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>3</v>
+        <v>53</v>
       </c>
       <c r="C2" s="7"/>
       <c r="D2" s="7"/>
@@ -946,10 +946,10 @@
       <c r="J2" s="7"/>
       <c r="K2" s="7"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="9"/>
       <c r="B3" s="7" t="s">
-        <v>4</v>
+        <v>71</v>
       </c>
       <c r="C3" s="7"/>
       <c r="D3" s="7"/>
@@ -961,281 +961,7 @@
       <c r="J3" s="7"/>
       <c r="K3" s="7"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="8"/>
-      <c r="D4" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="11"/>
-      <c r="B5" t="s">
-        <v>30</v>
-      </c>
-      <c r="F5" s="11" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="11"/>
-      <c r="C6" t="s">
-        <v>31</v>
-      </c>
-      <c r="E6" t="s">
-        <v>13</v>
-      </c>
-      <c r="F6" s="11"/>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="11"/>
-      <c r="C7" t="s">
-        <v>32</v>
-      </c>
-      <c r="E7" t="s">
-        <v>13</v>
-      </c>
-      <c r="F7" s="11"/>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="11"/>
-      <c r="C8" t="s">
-        <v>33</v>
-      </c>
-      <c r="E8" t="s">
-        <v>13</v>
-      </c>
-      <c r="F8" s="11"/>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="11"/>
-      <c r="C9" t="s">
-        <v>34</v>
-      </c>
-      <c r="E9" t="s">
-        <v>13</v>
-      </c>
-      <c r="F9" s="11"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="11"/>
-      <c r="C10" t="s">
-        <v>35</v>
-      </c>
-      <c r="E10" t="s">
-        <v>13</v>
-      </c>
-      <c r="F10" s="11"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="11"/>
-      <c r="C11" t="s">
-        <v>36</v>
-      </c>
-      <c r="E11" t="s">
-        <v>13</v>
-      </c>
-      <c r="F11" s="11"/>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="11"/>
-      <c r="C12" t="s">
-        <v>37</v>
-      </c>
-      <c r="E12" t="s">
-        <v>13</v>
-      </c>
-      <c r="F12" s="11"/>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="11"/>
-      <c r="C13" t="s">
-        <v>38</v>
-      </c>
-      <c r="F13" s="11"/>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="11"/>
-      <c r="C14" t="s">
-        <v>39</v>
-      </c>
-      <c r="F14" s="11"/>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="11"/>
-      <c r="F15" s="11"/>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="11"/>
-      <c r="F16" s="11"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="11"/>
-      <c r="F17" s="11"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="11"/>
-      <c r="F18" s="11"/>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="11"/>
-      <c r="F19" s="11"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="11"/>
-      <c r="B20" t="s">
-        <v>40</v>
-      </c>
-      <c r="F20" s="11"/>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="11"/>
-      <c r="F21" s="11"/>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="11"/>
-      <c r="F22" s="11"/>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="11"/>
-      <c r="F23" s="11"/>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="11"/>
-      <c r="F24" s="11"/>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="11"/>
-      <c r="B25" t="s">
-        <v>41</v>
-      </c>
-      <c r="F25" s="11"/>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="11"/>
-      <c r="C26" t="s">
-        <v>42</v>
-      </c>
-      <c r="E26" t="s">
-        <v>13</v>
-      </c>
-      <c r="F26" s="11"/>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="11"/>
-      <c r="C27" t="s">
-        <v>43</v>
-      </c>
-      <c r="E27" t="s">
-        <v>13</v>
-      </c>
-      <c r="F27" s="11"/>
-    </row>
-  </sheetData>
-  <mergeCells count="7">
-    <mergeCell ref="B1:K1"/>
-    <mergeCell ref="B2:K2"/>
-    <mergeCell ref="B3:K3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="A4:A27"/>
-    <mergeCell ref="F5:F27"/>
-  </mergeCells>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E5 E20 E25" xr:uid="{00000000-0002-0000-0100-000000000000}">
-      <formula1>"是,否"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E21 E22 E23 E24 E26 E27 E6:E12 E13:E17 E18:E19" xr:uid="{00000000-0002-0000-0100-000001000000}">
-      <formula1>"√,×"</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:K13"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="23.33203125" customWidth="1"/>
-    <col min="2" max="2" width="25" customWidth="1"/>
-    <col min="3" max="3" width="64.77734375" customWidth="1"/>
-    <col min="4" max="4" width="25.21875" customWidth="1"/>
-    <col min="5" max="5" width="18.21875" customWidth="1"/>
-    <col min="6" max="6" width="32.33203125" customWidth="1"/>
-    <col min="7" max="7" width="22.5546875" customWidth="1"/>
-    <col min="11" max="11" width="9" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:11" ht="31.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
-      <c r="J1" s="6"/>
-      <c r="K1" s="6"/>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7"/>
-      <c r="J2" s="7"/>
-      <c r="K2" s="7"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="9"/>
-      <c r="B3" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="7"/>
-      <c r="I3" s="7"/>
-      <c r="J3" s="7"/>
-      <c r="K3" s="7"/>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="10"/>
       <c r="B4" s="7" t="s">
         <v>4</v>
@@ -1250,7 +976,7 @@
       <c r="J4" s="7"/>
       <c r="K4" s="7"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="11" t="s">
         <v>5</v>
       </c>
@@ -1268,14 +994,14 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="11"/>
       <c r="B6" t="s">
         <v>72</v>
       </c>
       <c r="F6" s="11"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="11"/>
       <c r="C7" t="s">
         <v>74</v>
@@ -1285,7 +1011,7 @@
       </c>
       <c r="F7" s="11"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" s="11"/>
       <c r="C8" t="s">
         <v>75</v>
@@ -1295,7 +1021,7 @@
       </c>
       <c r="F8" s="11"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="11"/>
       <c r="C9" t="s">
         <v>76</v>
@@ -1305,16 +1031,16 @@
       </c>
       <c r="F9" s="11"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="F10" s="11"/>
     </row>
-    <row r="11" spans="1:11" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" ht="13.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
         <v>73</v>
       </c>
       <c r="F11" s="11"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="C12" t="s">
         <v>77</v>
       </c>
@@ -1323,7 +1049,7 @@
       </c>
       <c r="F12" s="11"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="F13" s="11"/>
     </row>
   </sheetData>
@@ -1339,10 +1065,10 @@
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E7:E13" xr:uid="{D7184A6A-6F18-46A8-AD24-31F8EC28EEB0}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E7:E13">
       <formula1>"√,×"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E6" xr:uid="{3DD9E351-C80C-4148-8D4F-BE7195DE58ED}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E6">
       <formula1>"是,否"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1350,30 +1076,31 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:K10"/>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15" customWidth="1"/>
-    <col min="2" max="2" width="22.44140625" customWidth="1"/>
-    <col min="3" max="3" width="57.109375" customWidth="1"/>
-    <col min="4" max="4" width="17.21875" customWidth="1"/>
-    <col min="5" max="5" width="18.5546875" customWidth="1"/>
-    <col min="6" max="6" width="20" customWidth="1"/>
+    <col min="1" max="1" width="12.75" customWidth="1"/>
+    <col min="2" max="2" width="40.4140625" customWidth="1"/>
+    <col min="3" max="3" width="67.08203125" customWidth="1"/>
+    <col min="4" max="4" width="15.4140625" customWidth="1"/>
+    <col min="5" max="5" width="16.75" customWidth="1"/>
+    <col min="6" max="6" width="30.4140625" customWidth="1"/>
+    <col min="13" max="15" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="37.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="C1" s="6"/>
       <c r="D1" s="6"/>
@@ -1385,10 +1112,12 @@
       <c r="J1" s="6"/>
       <c r="K1" s="6"/>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="2"/>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A2" s="9" t="s">
+        <v>2</v>
+      </c>
       <c r="B2" s="7" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C2" s="7"/>
       <c r="D2" s="7"/>
@@ -1400,7 +1129,277 @@
       <c r="J2" s="7"/>
       <c r="K2" s="7"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A3" s="9"/>
+      <c r="B3" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
+      <c r="J3" s="7"/>
+      <c r="K3" s="7"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A4" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="8"/>
+      <c r="D4" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A5" s="11"/>
+      <c r="B5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F5" s="11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A6" s="11"/>
+      <c r="C6" t="s">
+        <v>31</v>
+      </c>
+      <c r="E6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F6" s="11"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A7" s="11"/>
+      <c r="C7" t="s">
+        <v>32</v>
+      </c>
+      <c r="E7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F7" s="11"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A8" s="11"/>
+      <c r="C8" t="s">
+        <v>33</v>
+      </c>
+      <c r="E8" t="s">
+        <v>13</v>
+      </c>
+      <c r="F8" s="11"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A9" s="11"/>
+      <c r="C9" t="s">
+        <v>34</v>
+      </c>
+      <c r="E9" t="s">
+        <v>13</v>
+      </c>
+      <c r="F9" s="11"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A10" s="11"/>
+      <c r="C10" t="s">
+        <v>35</v>
+      </c>
+      <c r="E10" t="s">
+        <v>13</v>
+      </c>
+      <c r="F10" s="11"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A11" s="11"/>
+      <c r="C11" t="s">
+        <v>36</v>
+      </c>
+      <c r="E11" t="s">
+        <v>13</v>
+      </c>
+      <c r="F11" s="11"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A12" s="11"/>
+      <c r="C12" t="s">
+        <v>37</v>
+      </c>
+      <c r="E12" t="s">
+        <v>13</v>
+      </c>
+      <c r="F12" s="11"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A13" s="11"/>
+      <c r="C13" t="s">
+        <v>38</v>
+      </c>
+      <c r="F13" s="11"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A14" s="11"/>
+      <c r="C14" t="s">
+        <v>39</v>
+      </c>
+      <c r="F14" s="11"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A15" s="11"/>
+      <c r="F15" s="11"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A16" s="11"/>
+      <c r="F16" s="11"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" s="11"/>
+      <c r="F17" s="11"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" s="11"/>
+      <c r="F18" s="11"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19" s="11"/>
+      <c r="F19" s="11"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20" s="11"/>
+      <c r="B20" t="s">
+        <v>40</v>
+      </c>
+      <c r="F20" s="11"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A21" s="11"/>
+      <c r="F21" s="11"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A22" s="11"/>
+      <c r="F22" s="11"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A23" s="11"/>
+      <c r="F23" s="11"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A24" s="11"/>
+      <c r="F24" s="11"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A25" s="11"/>
+      <c r="B25" t="s">
+        <v>41</v>
+      </c>
+      <c r="F25" s="11"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A26" s="11"/>
+      <c r="C26" t="s">
+        <v>42</v>
+      </c>
+      <c r="E26" t="s">
+        <v>13</v>
+      </c>
+      <c r="F26" s="11"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A27" s="11"/>
+      <c r="C27" t="s">
+        <v>43</v>
+      </c>
+      <c r="E27" t="s">
+        <v>13</v>
+      </c>
+      <c r="F27" s="11"/>
+    </row>
+  </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="B1:K1"/>
+    <mergeCell ref="B2:K2"/>
+    <mergeCell ref="B3:K3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="A4:A27"/>
+    <mergeCell ref="F5:F27"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E5 E20 E25">
+      <formula1>"是,否"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E21 E22 E23 E24 E26 E27 E6:E12 E13:E17 E18:E19">
+      <formula1>"√,×"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="15" customWidth="1"/>
+    <col min="2" max="2" width="22.4140625" customWidth="1"/>
+    <col min="3" max="3" width="57.08203125" customWidth="1"/>
+    <col min="4" max="4" width="17.25" customWidth="1"/>
+    <col min="5" max="5" width="18.58203125" customWidth="1"/>
+    <col min="6" max="6" width="20" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="38" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="6"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A2" s="2"/>
+      <c r="B2" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
+      <c r="J2" s="7"/>
+      <c r="K2" s="7"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="11" t="s">
         <v>5</v>
       </c>
@@ -1418,14 +1417,14 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="11"/>
       <c r="B4" t="s">
         <v>45</v>
       </c>
       <c r="F4" s="11"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="11"/>
       <c r="C5" t="s">
         <v>46</v>
@@ -1435,7 +1434,7 @@
       </c>
       <c r="F5" s="11"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="11"/>
       <c r="C6" t="s">
         <v>47</v>
@@ -1445,7 +1444,7 @@
       </c>
       <c r="F6" s="11"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="11"/>
       <c r="C7" t="s">
         <v>48</v>
@@ -1455,7 +1454,7 @@
       </c>
       <c r="F7" s="11"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" s="11"/>
       <c r="C8" t="s">
         <v>49</v>
@@ -1465,7 +1464,7 @@
       </c>
       <c r="F8" s="11"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="11"/>
       <c r="C9" t="s">
         <v>50</v>
@@ -1475,7 +1474,7 @@
       </c>
       <c r="F9" s="11"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="11"/>
       <c r="C10" t="s">
         <v>51</v>
@@ -1495,10 +1494,10 @@
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E4" xr:uid="{00000000-0002-0000-0300-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E4">
       <formula1>"是,否"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E5:E7" xr:uid="{00000000-0002-0000-0300-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E5:E7">
       <formula1>"√,×"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1507,23 +1506,23 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.44140625" customWidth="1"/>
-    <col min="2" max="2" width="30.109375" customWidth="1"/>
+    <col min="1" max="1" width="22.4140625" customWidth="1"/>
+    <col min="2" max="2" width="30.08203125" customWidth="1"/>
     <col min="3" max="3" width="27" customWidth="1"/>
-    <col min="4" max="4" width="19.21875" customWidth="1"/>
-    <col min="6" max="6" width="24.88671875" customWidth="1"/>
+    <col min="4" max="4" width="19.25" customWidth="1"/>
+    <col min="6" max="6" width="24.9140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" ht="20" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1546,7 +1545,7 @@
       <c r="P1" s="4"/>
       <c r="Q1" s="4"/>
     </row>
-    <row r="2" spans="1:17" ht="13.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" ht="14" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
         <v>2</v>
       </c>
@@ -1569,7 +1568,7 @@
       <c r="P2" s="4"/>
       <c r="Q2" s="4"/>
     </row>
-    <row r="3" spans="1:17" ht="13.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" ht="14" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="10"/>
       <c r="B3" s="7" t="s">
         <v>4</v>
@@ -1588,7 +1587,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A4" s="11" t="s">
         <v>5</v>
       </c>
@@ -1606,14 +1605,14 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A5" s="11"/>
       <c r="B5" t="s">
         <v>55</v>
       </c>
       <c r="F5" s="11"/>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6" s="11"/>
       <c r="C6" t="s">
         <v>56</v>
@@ -1623,14 +1622,14 @@
       </c>
       <c r="F6" s="11"/>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A7" s="11"/>
       <c r="B7" t="s">
         <v>57</v>
       </c>
       <c r="F7" s="11"/>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A8" s="11"/>
       <c r="C8" t="s">
         <v>58</v>
@@ -1652,10 +1651,10 @@
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E5 E7" xr:uid="{00000000-0002-0000-0400-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E5 E7">
       <formula1>"是,否"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E6 E8" xr:uid="{00000000-0002-0000-0400-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E6 E8">
       <formula1>"√,×"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1664,22 +1663,22 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.77734375" customWidth="1"/>
-    <col min="2" max="2" width="32.77734375" customWidth="1"/>
-    <col min="3" max="3" width="32.44140625" customWidth="1"/>
-    <col min="6" max="6" width="47.77734375" customWidth="1"/>
+    <col min="1" max="1" width="12.75" customWidth="1"/>
+    <col min="2" max="2" width="32.75" customWidth="1"/>
+    <col min="3" max="3" width="32.4140625" customWidth="1"/>
+    <col min="6" max="6" width="47.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="46.05" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="46" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1696,7 +1695,7 @@
       <c r="J1" s="6"/>
       <c r="K1" s="6"/>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
         <v>2</v>
       </c>
@@ -1713,7 +1712,7 @@
       <c r="J2" s="7"/>
       <c r="K2" s="7"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="10"/>
       <c r="B3" s="7" t="s">
         <v>4</v>
@@ -1728,7 +1727,7 @@
       <c r="J3" s="7"/>
       <c r="K3" s="7"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="11" t="s">
         <v>5</v>
       </c>
@@ -1746,7 +1745,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="11"/>
       <c r="B5" t="s">
         <v>61</v>
@@ -1755,7 +1754,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="11"/>
       <c r="C6" t="s">
         <v>63</v>
@@ -1765,11 +1764,11 @@
       </c>
       <c r="F6" s="11"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="11"/>
       <c r="F7" s="11"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" s="11"/>
       <c r="F8" s="11"/>
     </row>
@@ -1785,10 +1784,10 @@
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E5 E7" xr:uid="{00000000-0002-0000-0500-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E5 E7">
       <formula1>"是,否"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E6 E8" xr:uid="{00000000-0002-0000-0500-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E6 E8">
       <formula1>"√,×"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1797,24 +1796,24 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K8"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B54" sqref="B54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="20.6640625" customWidth="1"/>
-    <col min="2" max="2" width="21.109375" customWidth="1"/>
+    <col min="2" max="2" width="21.08203125" customWidth="1"/>
     <col min="3" max="3" width="31.33203125" customWidth="1"/>
     <col min="4" max="4" width="17.33203125" customWidth="1"/>
-    <col min="5" max="5" width="20.44140625" customWidth="1"/>
-    <col min="6" max="6" width="26.77734375" customWidth="1"/>
+    <col min="5" max="5" width="20.4140625" customWidth="1"/>
+    <col min="6" max="6" width="26.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="42.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="42.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1831,7 +1830,7 @@
       <c r="J1" s="6"/>
       <c r="K1" s="6"/>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
         <v>2</v>
       </c>
@@ -1848,7 +1847,7 @@
       <c r="J2" s="7"/>
       <c r="K2" s="7"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="10"/>
       <c r="B3" s="7" t="s">
         <v>4</v>
@@ -1863,7 +1862,7 @@
       <c r="J3" s="7"/>
       <c r="K3" s="7"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="11" t="s">
         <v>5</v>
       </c>
@@ -1881,7 +1880,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="11"/>
       <c r="B5" t="s">
         <v>55</v>
@@ -1890,7 +1889,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="11"/>
       <c r="C6" t="s">
         <v>67</v>
@@ -1900,7 +1899,7 @@
       </c>
       <c r="F6" s="11"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="11"/>
       <c r="C7" t="s">
         <v>68</v>
@@ -1910,7 +1909,7 @@
       </c>
       <c r="F7" s="11"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" s="11"/>
       <c r="C8" t="s">
         <v>69</v>
@@ -1932,10 +1931,10 @@
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E5" xr:uid="{00000000-0002-0000-0600-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E5">
       <formula1>"是,否"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E6:E8" xr:uid="{00000000-0002-0000-0600-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E6:E8">
       <formula1>"√,×"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>